<commit_message>
Added CIL & Test Strategy
</commit_message>
<xml_diff>
--- a/PM/CIL/CIL.xlsx
+++ b/PM/CIL/CIL.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Alaa Osama\Documents\GitHub\learning-hub\PM\CIL\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C73C853C-15B9-4971-8BDC-87BDD6387BBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -16,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t xml:space="preserve">Configuration Item List </t>
   </si>
@@ -51,9 +57,6 @@
     <t>RTM</t>
   </si>
   <si>
-    <t>https://github.com/AlaaOsama25/learning-hub/blob/main/PM/PMP/RTM.xlsx</t>
-  </si>
-  <si>
     <t>https://github.com/AlaaOsama25/learning-hub/blob/main/PM/CIL/CIL.xlsx</t>
   </si>
   <si>
@@ -69,9 +72,6 @@
     <t>CRS</t>
   </si>
   <si>
-    <t>https://github.com/AlaaOsama25/learning-hub/blob/main/Requirements/SRS/SRS_login_register.docx</t>
-  </si>
-  <si>
     <t xml:space="preserve">Requirements Review Sheet </t>
   </si>
   <si>
@@ -103,12 +103,42 @@
   </si>
   <si>
     <t>Test Review Sheet</t>
+  </si>
+  <si>
+    <t>https://github.com/AlaaOsama25/learning-hub/blob/main/PM/Schedule/Scheduling.xlsx</t>
+  </si>
+  <si>
+    <t>WBS</t>
+  </si>
+  <si>
+    <t>https://github.com/AlaaOsama25/learning-hub/blob/main/PM/Schedule/WBS.xlsx</t>
+  </si>
+  <si>
+    <t>RACI</t>
+  </si>
+  <si>
+    <t>https://github.com/AlaaOsama25/learning-hub/blob/main/PM/RACI-Matrix.xlsx</t>
+  </si>
+  <si>
+    <t>https://github.com/AlaaOsama25/learning-hub/blob/main/Requirements/CRS/CRS.xlsx</t>
+  </si>
+  <si>
+    <t>https://github.com/AlaaOsama25/learning-hub/tree/main/Requirements/SIQ</t>
+  </si>
+  <si>
+    <t>https://github.com/AlaaOsama25/learning-hub/tree/main/Requirements/SRS</t>
+  </si>
+  <si>
+    <t>https://github.com/AlaaOsama25/learning-hub/tree/main/Design/Diagrams</t>
+  </si>
+  <si>
+    <t>Test Strategy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -305,22 +335,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyBorder="1"/>
@@ -328,12 +346,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -343,6 +355,30 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -354,6 +390,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -402,7 +441,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -435,9 +474,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -470,6 +526,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -645,222 +718,253 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="33.140625" style="15" customWidth="1"/>
-    <col min="2" max="2" width="96.5703125" customWidth="1"/>
-    <col min="3" max="3" width="26.7109375" customWidth="1"/>
+    <col min="1" max="1" width="33.109375" style="9" customWidth="1"/>
+    <col min="2" max="2" width="96.5546875" customWidth="1"/>
+    <col min="3" max="3" width="26.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="1" customFormat="1" ht="36" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:2" s="1" customFormat="1" ht="36.6" x14ac:dyDescent="0.7">
+      <c r="A1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3"/>
-    </row>
-    <row r="2" spans="1:2" ht="21" x14ac:dyDescent="0.35">
-      <c r="A2" s="13" t="s">
+      <c r="B1" s="13"/>
+    </row>
+    <row r="2" spans="1:2" ht="21" x14ac:dyDescent="0.4">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:2" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="A3" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="6"/>
-    </row>
-    <row r="4" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A4" s="14" t="s">
+      <c r="B3" s="11"/>
+    </row>
+    <row r="4" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A4" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A5" s="14" t="s">
+    <row r="5" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A5" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="3"/>
+    </row>
+    <row r="6" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A6" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A6" s="14" t="s">
-        <v>7</v>
-      </c>
-      <c r="B6" s="7" t="s">
+    <row r="7" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A7" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A8" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A9" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A10" s="8" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A7" s="14" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="8"/>
-    </row>
-    <row r="8" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A8" s="14" t="s">
+      <c r="B10" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="9" t="s">
+    </row>
+    <row r="11" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A11" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="17"/>
+    </row>
+    <row r="12" spans="1:2" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="A12" s="14" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A9" s="10" t="s">
+      <c r="B12" s="15"/>
+    </row>
+    <row r="13" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A13" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="11"/>
-    </row>
-    <row r="10" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A10" s="14" t="s">
+      <c r="B13" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A14" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A15" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A16" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="B10" s="8"/>
-    </row>
-    <row r="11" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="B11" s="8"/>
-    </row>
-    <row r="12" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A12" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" s="7" t="s">
+      <c r="B16" s="4"/>
+    </row>
+    <row r="17" spans="1:2" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="A17" s="10" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A13" s="14" t="s">
+      <c r="B17" s="11"/>
+    </row>
+    <row r="18" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A18" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="8"/>
-    </row>
-    <row r="14" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A14" s="5" t="s">
+      <c r="B18" s="4"/>
+    </row>
+    <row r="19" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A19" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="6"/>
-    </row>
-    <row r="15" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="14" t="s">
+      <c r="B19" s="4"/>
+    </row>
+    <row r="20" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A20" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="8"/>
-    </row>
-    <row r="16" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A16" s="14" t="s">
+      <c r="B20" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="A21" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="8"/>
-    </row>
-    <row r="17" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A17" s="14" t="s">
+      <c r="B21" s="11"/>
+    </row>
+    <row r="22" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A22" s="8"/>
+      <c r="B22" s="4"/>
+    </row>
+    <row r="23" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A23" s="8"/>
+      <c r="B23" s="4"/>
+    </row>
+    <row r="24" spans="1:2" ht="25.8" x14ac:dyDescent="0.5">
+      <c r="A24" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B17" s="8"/>
-    </row>
-    <row r="18" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A18" s="5" t="s">
+      <c r="B24" s="11"/>
+    </row>
+    <row r="25" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A25" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B18" s="6"/>
-    </row>
-    <row r="19" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="14"/>
-      <c r="B19" s="8"/>
-    </row>
-    <row r="20" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A20" s="14"/>
-      <c r="B20" s="8"/>
-    </row>
-    <row r="21" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
-      <c r="A21" s="5" t="s">
+      <c r="B25" s="4"/>
+    </row>
+    <row r="26" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A26" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="6"/>
-    </row>
-    <row r="22" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A22" s="14" t="s">
+      <c r="B26" s="4"/>
+    </row>
+    <row r="27" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A27" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="B22" s="8"/>
-    </row>
-    <row r="23" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A23" s="14" t="s">
+      <c r="B27" s="4"/>
+    </row>
+    <row r="28" spans="1:2" ht="18" x14ac:dyDescent="0.35">
+      <c r="A28" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B23" s="8"/>
-    </row>
-    <row r="24" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A24" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="B24" s="8"/>
-    </row>
-    <row r="25" spans="1:2" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A25" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="B25" s="8"/>
-    </row>
-    <row r="26" spans="1:2" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="14"/>
-      <c r="B26" s="12"/>
+      <c r="B28" s="4"/>
+    </row>
+    <row r="29" spans="1:2" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A29" s="8"/>
+      <c r="B29" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A24:B24"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A21:B21"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B8" r:id="rId1"/>
-    <hyperlink ref="B4" r:id="rId2"/>
-    <hyperlink ref="B5" r:id="rId3"/>
-    <hyperlink ref="B6" r:id="rId4"/>
-    <hyperlink ref="B12" r:id="rId5"/>
+    <hyperlink ref="B10" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="B4" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="B6" r:id="rId3" xr:uid="{00000000-0004-0000-0000-000002000000}"/>
+    <hyperlink ref="B15" r:id="rId4" display="https://github.com/AlaaOsama25/learning-hub/blob/main/Requirements/SRS/SRS_login_register.docx" xr:uid="{00000000-0004-0000-0000-000003000000}"/>
+    <hyperlink ref="B9" r:id="rId5" xr:uid="{00000000-0004-0000-0000-000004000000}"/>
+    <hyperlink ref="B7" r:id="rId6" xr:uid="{00000000-0004-0000-0000-000005000000}"/>
+    <hyperlink ref="B13" r:id="rId7" xr:uid="{00000000-0004-0000-0000-000006000000}"/>
+    <hyperlink ref="B20" r:id="rId8" xr:uid="{E4CF924D-08DF-4F60-9960-82AA938AD9D4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId9"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>